<commit_message>
new sheet -Log- is added to report
</commit_message>
<xml_diff>
--- a/bin/com/styletag/test_cases/TestSuit.xlsx
+++ b/bin/com/styletag/test_cases/TestSuit.xlsx
@@ -46,10 +46,10 @@
     <t xml:space="preserve">NO</t>
   </si>
   <si>
-    <t xml:space="preserve">login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">logout</t>
+    <t xml:space="preserve">productCatalogPage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">applyFilters</t>
   </si>
   <si>
     <t xml:space="preserve">Search</t>
@@ -187,15 +187,16 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>